<commit_message>
Cambio en el PractitionerRole
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-CoreMedicamentoCl.xlsx
+++ b/output/StructureDefinition-CoreMedicamentoCl.xlsx
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-07-18T16:07:51-04:00</t>
+    <t>2024-07-26T10:55:50-04:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -1188,36 +1188,37 @@
     <t>Medication.ingredient.item[x]</t>
   </si>
   <si>
+    <t>CodeableConcept
+Reference(Substance|Medication)</t>
+  </si>
+  <si>
+    <t>The actual ingredient or content</t>
+  </si>
+  <si>
+    <t>The actual ingredient - either a substance (simple ingredient) or another medication of a medication.</t>
+  </si>
+  <si>
+    <t>The ingredient may reference a substance (for example, amoxicillin) or another medication (for example in the case of a compounded product, Glaxal Base).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">type:$this}
+</t>
+  </si>
+  <si>
+    <t>.player</t>
+  </si>
+  <si>
+    <t>RXC-2-Component Code  if medication: RXO-1-Requested Give Code / RXE-2-Give Code / RXD-2-Dispense/Give Code / RXG-4-Give Code / RXA-5-Administered Code</t>
+  </si>
+  <si>
+    <t>Medication.ingredient.item[x]:itemReference</t>
+  </si>
+  <si>
+    <t>itemReference</t>
+  </si>
+  <si>
     <t xml:space="preserve">Reference(Substance|Medication)
 </t>
-  </si>
-  <si>
-    <t>The actual ingredient or content</t>
-  </si>
-  <si>
-    <t>The actual ingredient - either a substance (simple ingredient) or another medication of a medication.</t>
-  </si>
-  <si>
-    <t>The ingredient may reference a substance (for example, amoxicillin) or another medication (for example in the case of a compounded product, Glaxal Base).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">type:$this}
-</t>
-  </si>
-  <si>
-    <t>closed</t>
-  </si>
-  <si>
-    <t>.player</t>
-  </si>
-  <si>
-    <t>RXC-2-Component Code  if medication: RXO-1-Requested Give Code / RXE-2-Give Code / RXD-2-Dispense/Give Code / RXG-4-Give Code / RXA-5-Administered Code</t>
-  </si>
-  <si>
-    <t>Medication.ingredient.item[x]:itemReference</t>
-  </si>
-  <si>
-    <t>itemReference</t>
   </si>
   <si>
     <t>Componente del fármaco, se usará texto</t>
@@ -10206,7 +10207,7 @@
         <v>78</v>
       </c>
       <c r="AE73" t="s" s="2">
-        <v>380</v>
+        <v>137</v>
       </c>
       <c r="AF73" t="s" s="2">
         <v>374</v>
@@ -10227,31 +10228,31 @@
         <v>304</v>
       </c>
       <c r="AL73" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="AM73" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AN73" t="s" s="2">
         <v>381</v>
-      </c>
-      <c r="AM73" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AN73" t="s" s="2">
-        <v>382</v>
       </c>
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B74" t="s" s="2">
         <v>374</v>
       </c>
       <c r="C74" t="s" s="2">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D74" t="s" s="2">
         <v>78</v>
       </c>
       <c r="E74" s="2"/>
       <c r="F74" t="s" s="2">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="G74" t="s" s="2">
         <v>88</v>
@@ -10266,7 +10267,7 @@
         <v>78</v>
       </c>
       <c r="K74" t="s" s="2">
-        <v>375</v>
+        <v>384</v>
       </c>
       <c r="L74" t="s" s="2">
         <v>385</v>
@@ -10343,13 +10344,13 @@
         <v>304</v>
       </c>
       <c r="AL74" t="s" s="2">
+        <v>380</v>
+      </c>
+      <c r="AM74" t="s" s="2">
+        <v>78</v>
+      </c>
+      <c r="AN74" t="s" s="2">
         <v>381</v>
-      </c>
-      <c r="AM74" t="s" s="2">
-        <v>78</v>
-      </c>
-      <c r="AN74" t="s" s="2">
-        <v>382</v>
       </c>
     </row>
     <row r="75" hidden="true">

</xml_diff>

<commit_message>
Agregar CapabilityStatement y orden de la guía
</commit_message>
<xml_diff>
--- a/output/StructureDefinition-CoreMedicamentoCl.xlsx
+++ b/output/StructureDefinition-CoreMedicamentoCl.xlsx
@@ -45,7 +45,7 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Medicamento Core CL</t>
+    <t>CL Medicamento</t>
   </si>
   <si>
     <t>Status</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-08-06T16:31:07-04:00</t>
+    <t>2024-08-07T09:55:47-04:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>